<commit_message>
GERD turbine flow corrected
</commit_message>
<xml_diff>
--- a/nile_EMODPS_framework/settings/settings_file_Nile.xlsx
+++ b/nile_EMODPS_framework/settings/settings_file_Nile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yasinsari/Documents/master-thesis-project/Nile_EMODPS_framework/settings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yasinsari/Documents/master-thesis-project/nile_EMODPS_framework/settings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F5240C-0C12-B447-9A17-8061047EB8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B45477-B86F-7C48-9C59-FB9F8895CC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15580" activeTab="1" xr2:uid="{65B2DD87-E74E-094B-8E0A-FAA834E63631}"/>
+    <workbookView xWindow="-27860" yWindow="3400" windowWidth="27860" windowHeight="15580" xr2:uid="{65B2DD87-E74E-094B-8E0A-FAA834E63631}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelParameters" sheetId="4" r:id="rId1"/>
@@ -270,9 +270,6 @@
     <t>[0.90]</t>
   </si>
   <si>
-    <t>[0.75]</t>
-  </si>
-  <si>
     <t>[0.60]</t>
   </si>
   <si>
@@ -303,7 +300,10 @@
     <t>half-an-hour</t>
   </si>
   <si>
-    <t>[2544]</t>
+    <t>[0.93]</t>
+  </si>
+  <si>
+    <t>[4320]</t>
   </si>
 </sst>
 </file>
@@ -712,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10871A19-541A-E94D-BB27-74C5363B6884}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -831,7 +831,7 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -865,7 +865,7 @@
         <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -879,16 +879,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10">
         <v>5</v>
       </c>
       <c r="C10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" t="s">
         <v>85</v>
-      </c>
-      <c r="D10" t="s">
-        <v>86</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
@@ -903,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C46D96C-8ADA-8E40-B2A8-24351E5FCFAE}">
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -946,7 +946,7 @@
         <v>58</v>
       </c>
       <c r="B2" s="10">
-        <v>5000000000</v>
+        <v>10000000000</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
@@ -955,7 +955,7 @@
         <v>88</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>63</v>
@@ -966,7 +966,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="6">
         <v>4571250000</v>
@@ -978,7 +978,7 @@
         <v>75</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>64</v>
@@ -1001,7 +1001,7 @@
         <v>72</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>65</v>
@@ -1295,7 +1295,7 @@
         <v>37</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
         <v>49</v>
@@ -1309,7 +1309,7 @@
         <v>38</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D8" t="s">
         <v>50</v>
@@ -1323,7 +1323,7 @@
         <v>39</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D9" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
Resimulation with TWh and growth
</commit_message>
<xml_diff>
--- a/nile_EMODPS_framework/settings/settings_file_Nile.xlsx
+++ b/nile_EMODPS_framework/settings/settings_file_Nile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yasinsari/Documents/master-thesis-project/nile_EMODPS_framework/settings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824C5364-CCB2-6E41-978B-06DC378C7473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A064C34C-1A36-5B49-B070-7F9BE6A431BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27860" yWindow="3400" windowWidth="27860" windowHeight="15580" xr2:uid="{65B2DD87-E74E-094B-8E0A-FAA834E63631}"/>
+    <workbookView xWindow="-27860" yWindow="3400" windowWidth="27860" windowHeight="15580" activeTab="1" xr2:uid="{65B2DD87-E74E-094B-8E0A-FAA834E63631}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelParameters" sheetId="4" r:id="rId1"/>
@@ -228,9 +228,6 @@
     <t>["USSennar", "Gezira", "DSSennar", "Taminiat", "Hassanab", "Egypt"]</t>
   </si>
   <si>
-    <t>[590]</t>
-  </si>
-  <si>
     <t>[467]</t>
   </si>
   <si>
@@ -304,6 +301,9 @@
   </si>
   <si>
     <t>[4320]</t>
+  </si>
+  <si>
+    <t>[507]</t>
   </si>
 </sst>
 </file>
@@ -712,7 +712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10871A19-541A-E94D-BB27-74C5363B6884}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -831,7 +831,7 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -865,7 +865,7 @@
         <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -879,16 +879,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B10">
         <v>5</v>
       </c>
       <c r="C10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" t="s">
         <v>84</v>
-      </c>
-      <c r="D10" t="s">
-        <v>85</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
@@ -903,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C46D96C-8ADA-8E40-B2A8-24351E5FCFAE}">
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -938,7 +938,7 @@
         <v>26</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -952,21 +952,21 @@
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="G2" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" s="6">
         <v>4571250000</v>
@@ -975,16 +975,16 @@
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -998,16 +998,16 @@
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1021,21 +1021,21 @@
         <v>1</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.2">
@@ -1295,7 +1295,7 @@
         <v>37</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D7" t="s">
         <v>49</v>
@@ -1309,7 +1309,7 @@
         <v>38</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
         <v>50</v>
@@ -1323,7 +1323,7 @@
         <v>39</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D9" t="s">
         <v>51</v>

</xml_diff>